<commit_message>
Various data and text fixes, as requested.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_remote_overcrowding_uploader/housing_remote_overcrowding.xlsx
+++ b/dashboard_loader/housing_remote_overcrowding_uploader/housing_remote_overcrowding.xlsx
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Overcrowding places stress on household infrastructure such as food preparation areas and ablution systems. This can impact people’s physical and mental health, through disease, chronic infection and social stress. In turn, these issues may affect a person’s ability to participate in education and employment. Severe overcrowding was the most common form of homelessness for Indigenous people living in remote Australia.</t>
   </si>
   <si>
-    <t xml:space="preserve">Data from the 2014-15 National Aboriginal and Torres Strait Islander Social Survey (NATSISS) shows the proportion of Aboriginal and Torres Strait Islanders reporting living in overcrowded houses in remote areas has decreased from 48% to 38% in the 2008 survey.</t>
+    <t xml:space="preserve">Data from the 2014-15 National Aboriginal and Torres Strait Islander Social Survey (NATSISS) shows the proportion of Aboriginal and Torres Strait Islanders reporting living in overcrowded houses in remote areas has decreased to 38% from 48% in the 2008 survey.</t>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
@@ -117,11 +117,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -156,12 +157,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -248,7 +243,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,15 +327,15 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="57.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,15 +396,15 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="94.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="94.2"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,7 +439,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -452,7 +447,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
         <v>15</v>
@@ -475,7 +470,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>